<commit_message>
Dodanie rozdzialu o wplywie rodzaju ekspalntatu na ilosc otrzymanych regeneratow
</commit_message>
<xml_diff>
--- a/Wplyw rodzaju eksplantatu na efektywnosc regeneracyjna.xlsx
+++ b/Wplyw rodzaju eksplantatu na efektywnosc regeneracyjna.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Ogrodnictwo\Zaoczne\Praca inżynierska\InzynierkaOgro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Ogrodnictwo\Zaoczne\Praca inżynierska\InzynierkaOgro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1670C6EC-A80B-419B-8995-B49FA31C985C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7CFEEA-E0CA-48A3-8A62-0E421DF9B9A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rodzaj eksplant na efekt" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -316,7 +316,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$F$1</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -395,7 +395,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$5:$B$9</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$B$5:$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -418,7 +418,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$F$5:$F$9</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$F$5:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -451,7 +451,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$1</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -530,7 +530,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$5:$B$9</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$B$5:$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -553,7 +553,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$G$5:$G$9</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$G$5:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -945,7 +945,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$F$1</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1024,7 +1024,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$2:$B$4</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$B$2:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1041,7 +1041,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$F$2:$F$4</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1068,7 +1068,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$1</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1147,7 +1147,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$2:$B$4</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$B$2:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1164,7 +1164,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$G$2:$G$4</c:f>
+              <c:f>'Rodzaj eksplant na efekt'!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2960,7 +2960,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>